<commit_message>
Overall update of 3D models
</commit_message>
<xml_diff>
--- a/Structural parts/QuotationSet/Quotations.xlsx
+++ b/Structural parts/QuotationSet/Quotations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
-  <si>
-    <t>Fabnami</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Company</t>
   </si>
@@ -122,6 +119,15 @@
   </si>
   <si>
     <t>https://www.weerg.com/en/order</t>
+  </si>
+  <si>
+    <t>The 3D Printer Experience</t>
+  </si>
+  <si>
+    <t>All3dp.com</t>
+  </si>
+  <si>
+    <t>Greg</t>
   </si>
 </sst>
 </file>
@@ -165,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -189,19 +195,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -385,10 +378,105 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -402,33 +490,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
@@ -740,440 +848,486 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.140625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="16.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="13.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="16.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="11" max="11" width="88.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="12">
+      <c r="A2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="15">
         <v>205</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="3">
         <f>B2*$B$15</f>
         <v>180.4</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="16">
         <f>B2*$B$17</f>
         <v>57400</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="28">
         <v>18011</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="3">
         <f>E2*$B$15</f>
         <v>15849.68</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="16">
         <f>E2*$B$17</f>
         <v>5043080</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="24">
         <f>E2/100</f>
         <v>180.11</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="3">
         <f t="shared" ref="I2:J2" si="0">F2/100</f>
         <v>158.49680000000001</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="25">
         <f t="shared" si="0"/>
         <v>50430.8</v>
       </c>
-      <c r="K2" s="10" t="s">
-        <v>10</v>
+      <c r="K2" s="32" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="16">
+      <c r="A3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17">
         <f>D3*$B$18</f>
         <v>518.4</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="5">
         <f>D3*$B$20</f>
         <v>446.4</v>
       </c>
       <c r="D3" s="18">
         <v>144000</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="17">
         <f>G3*$B$18</f>
         <v>15840</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="5">
         <f>G3*$B$20</f>
         <v>13640</v>
       </c>
       <c r="G3" s="18">
         <v>4400000</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="24">
         <f t="shared" ref="H3:H7" si="1">E3/100</f>
         <v>158.4</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="3">
         <f t="shared" ref="I3:I7" si="2">F3/100</f>
         <v>136.4</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="25">
         <f t="shared" ref="J3:J7" si="3">G3/100</f>
         <v>44000</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="16">
+      <c r="A4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="17">
         <f>D4*$B$18</f>
         <v>396</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="5">
         <f>D4*$B$20</f>
         <v>341</v>
       </c>
       <c r="D4" s="18">
         <v>110000</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="17">
         <f>G4*$B$18</f>
         <v>20520</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="5">
         <f>G4*$B$20</f>
         <v>17670</v>
       </c>
       <c r="G4" s="18">
         <v>5700000</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="24">
         <f t="shared" si="1"/>
         <v>205.2</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="3">
         <f t="shared" si="2"/>
         <v>176.7</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="25">
         <f t="shared" si="3"/>
         <v>57000</v>
       </c>
-      <c r="K4" s="3"/>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="16">
+      <c r="A5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="17">
         <f>C5*$B$16</f>
         <v>712.49999999999989</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="6">
         <v>625</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="19">
         <f>C5*$B$19</f>
         <v>198806.24999999997</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="17">
         <f>F5*$B$16</f>
         <v>19950</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="6">
         <v>17500</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="19">
         <f>F5*$B$19</f>
         <v>5566575</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="24">
         <f t="shared" si="1"/>
         <v>199.5</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="3">
         <f t="shared" si="2"/>
         <v>175</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="25">
         <f t="shared" si="3"/>
         <v>55665.75</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="13">
+      <c r="A6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K6" s="11" t="s">
-        <v>27</v>
+      <c r="K6" s="34" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="16">
+      <c r="A7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="17">
         <f>C7*$B$16</f>
         <v>406.97999999999996</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="7">
         <v>357</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="19">
         <f>C7*$B$19</f>
         <v>113558.12999999999</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="17">
         <f>F7*$B$16</f>
-        <v>5736.48</v>
-      </c>
-      <c r="F7" s="18">
-        <v>5032</v>
-      </c>
-      <c r="G7" s="17">
+        <v>13950.179999999998</v>
+      </c>
+      <c r="F7" s="6">
+        <v>12237</v>
+      </c>
+      <c r="G7" s="19">
         <f>F7*$B$19</f>
-        <v>1600628.88</v>
-      </c>
-      <c r="H7" s="13">
+        <v>3892467.3299999996</v>
+      </c>
+      <c r="H7" s="24">
         <f t="shared" si="1"/>
-        <v>57.364799999999995</v>
-      </c>
-      <c r="I7" s="13">
+        <v>139.50179999999997</v>
+      </c>
+      <c r="I7" s="3">
         <f t="shared" si="2"/>
-        <v>50.32</v>
-      </c>
-      <c r="J7" s="13">
+        <v>122.37</v>
+      </c>
+      <c r="J7" s="25">
         <f t="shared" si="3"/>
-        <v>16006.288799999998</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>15</v>
+        <v>38924.673299999995</v>
+      </c>
+      <c r="K7" s="34" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="13">
+      <c r="A8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="24">
         <f t="shared" ref="H8:H9" si="4">E8/100</f>
         <v>0</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="3">
         <f t="shared" ref="I8:I9" si="5">F8/100</f>
         <v>0</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="25">
         <f t="shared" ref="J8:J9" si="6">G8/100</f>
         <v>0</v>
       </c>
-      <c r="K8" s="11" t="s">
-        <v>26</v>
+      <c r="K8" s="34" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="19">
+      <c r="A9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="20">
         <v>325</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="3">
         <f>B9*$B$15</f>
         <v>286</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="16">
         <f>B9*$B$17</f>
         <v>91000</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="29">
         <v>19327</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="3">
         <f>E9*$B$15</f>
         <v>17007.759999999998</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="16">
         <f>E9*$B$17</f>
         <v>5411560</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="24">
         <f t="shared" si="4"/>
         <v>193.27</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="3">
         <f t="shared" si="5"/>
         <v>170.07759999999999</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="25">
         <f t="shared" si="6"/>
         <v>54115.6</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="16">
+      <c r="B10" s="17">
         <f>C10*$B$16</f>
         <v>402.41999999999996</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="6">
         <v>353</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="19">
         <f>C10*$B$19</f>
         <v>112285.76999999999</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="17">
         <f>F10*$B$16</f>
         <v>24794.999999999996</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="6">
         <v>21750</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="19">
         <f>F10*$B$19</f>
         <v>6918457.4999999991</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="24">
         <f t="shared" ref="H10" si="7">E10/100</f>
         <v>247.94999999999996</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="3">
         <f t="shared" ref="I10" si="8">F10/100</f>
         <v>217.5</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="25">
         <f t="shared" ref="J10" si="9">G10/100</f>
         <v>69184.574999999997</v>
       </c>
-      <c r="K10" s="3"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="11" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="3"/>
+      <c r="A12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="20">
+        <v>130</v>
+      </c>
+      <c r="C12" s="4">
+        <f>B12*$B$15</f>
+        <v>114.4</v>
+      </c>
+      <c r="D12" s="19">
+        <f>B12*$B$17</f>
+        <v>36400</v>
+      </c>
+      <c r="E12" s="20">
+        <v>11800</v>
+      </c>
+      <c r="F12" s="4">
+        <f>E12*$B$15</f>
+        <v>10384</v>
+      </c>
+      <c r="G12" s="19">
+        <f>E12*$B$17</f>
+        <v>3304000</v>
+      </c>
+      <c r="H12" s="17">
+        <f t="shared" ref="H12" si="10">E12/100</f>
+        <v>118</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" ref="I12" si="11">F12/100</f>
+        <v>103.84</v>
+      </c>
+      <c r="J12" s="19">
+        <f t="shared" ref="J12" si="12">G12/100</f>
+        <v>33040</v>
+      </c>
+      <c r="K12" s="33"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="5"/>
+      <c r="A13" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="30">
+        <v>26100</v>
+      </c>
+      <c r="F13" s="8">
+        <f>E13*$B$15</f>
+        <v>22968</v>
+      </c>
+      <c r="G13" s="22">
+        <f>E13*$B$17</f>
+        <v>7308000</v>
+      </c>
+      <c r="H13" s="27">
+        <f t="shared" ref="H13" si="13">E13/100</f>
+        <v>261</v>
+      </c>
+      <c r="I13" s="8">
+        <f t="shared" ref="I13" si="14">F13/100</f>
+        <v>229.68</v>
+      </c>
+      <c r="J13" s="22">
+        <f t="shared" ref="J13" si="15">G13/100</f>
+        <v>73080</v>
+      </c>
+      <c r="K13" s="35"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>0.88</v>
@@ -1181,7 +1335,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>1.1399999999999999</v>
@@ -1189,7 +1343,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>280</v>
@@ -1197,7 +1351,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>3.5999999999999999E-3</v>
@@ -1205,7 +1359,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>318.08999999999997</v>
@@ -1213,7 +1367,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>3.0999999999999999E-3</v>

</xml_diff>